<commit_message>
change req to assets
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -1,13 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -26,7 +25,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
@@ -55,10 +59,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -78,7 +91,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -453,14 +466,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -639,9 +652,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix locale to FR with ,00 + fix merge
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -166,8 +166,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H4" headerRowCount="1">
-  <autoFilter ref="A1:H4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H2" headerRowCount="1">
+  <autoFilter ref="A1:H2"/>
   <tableColumns count="8">
     <tableColumn id="1" name="FILIALE"/>
     <tableColumn id="2" name="RESEAU"/>
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,21 +544,21 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>72681594150101332418418</t>
+          <t>72681594290101470231590</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>059369</t>
+          <t>143639</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-05-28</t>
+          <t>2024-10-15</t>
         </is>
       </c>
       <c r="F2" s="4" t="n">
-        <v>84000</v>
+        <v>92600</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -567,87 +567,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000118 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000118 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SG - COTE D IVOIRE</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>MASTERCARD INTERNATIONAL</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>72681594150101332421271</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>059347</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>25000</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>XOF</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000124 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000124 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>SG - COTE D IVOIRE</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>MASTERCARD INTERNATIONAL</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>72681594150101332383190</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>059403</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>435000</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>XOF</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000258 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000258 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
+          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000002 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000002 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
handle visa without recycled
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -166,8 +166,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H2" headerRowCount="1">
-  <autoFilter ref="A1:H2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H4" headerRowCount="1">
+  <autoFilter ref="A1:H4"/>
   <tableColumns count="8">
     <tableColumn id="1" name="FILIALE"/>
     <tableColumn id="2" name="RESEAU"/>
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,21 +544,21 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>72681594290101470231590</t>
+          <t>72681594150101332418418</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>143639</t>
+          <t>059369</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024-10-15</t>
+          <t>2024-05-28</t>
         </is>
       </c>
       <c r="F2" s="4" t="n">
-        <v>92600</v>
+        <v>84000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -567,7 +567,87 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000002 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000002 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
+          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000118 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000118 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SG - COTE D IVOIRE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>72681594150101332421271</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>059347</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-05-28</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>25000</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>XOF</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000124 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000124 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SG - COTE D IVOIRE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MASTERCARD INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>72681594150101332383190</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>059403</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-05-28</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>435000</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>XOF</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>COUNTRY CODE INVALID FOR BUSINESS SERVICE ARRANGEMENT 4384001 AND ACCEPTANCE BRAND ID CODE 00000258 D0043 S06 DMC. INTERCHANGE RATE DESIGNATOR AND PROCESSING CODE/REVERSAL INDICATOR COMBINATION INVALID FOR 00000258 P0158 S04 BUSINESS SERVICE ARRANGEMENT 2060001 AND ACCEPTANCE BRAND ID CODE DMC.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
handle reconciliation merge with recycle ok
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -33,7 +33,7 @@
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
@@ -43,12 +43,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="004F81BD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ffe26b0a"/>
-        <bgColor rgb="ffe26b0a"/>
       </patternFill>
     </fill>
   </fills>
@@ -70,7 +64,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -82,8 +76,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -162,8 +154,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L13" headerRowCount="1">
-  <autoFilter ref="A1:L13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L14" headerRowCount="1">
+  <autoFilter ref="A1:L14"/>
   <tableColumns count="12">
     <tableColumn id="1" name="FILIALE"/>
     <tableColumn id="2" name="Réseau"/>
@@ -471,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,58 +548,58 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>SG - BENIN</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>VISA INTERNATIONAL</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>ACHAT</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
-        <is>
-          <t>17-DEC-24</t>
-        </is>
-      </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>26-DEC-24</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>XOF</t>
         </is>
       </c>
-      <c r="F2" s="5" t="n">
-        <v>185</v>
-      </c>
-      <c r="G2" s="6" t="inlineStr">
-        <is>
-          <t>11827276.0</t>
+      <c r="F2" t="n">
+        <v>87</v>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>12062828.0</t>
         </is>
       </c>
       <c r="H2" s="5" t="inlineStr">
         <is>
-          <t>not ok</t>
-        </is>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="6" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>184</v>
-      </c>
-      <c r="L2" s="6" t="inlineStr">
-        <is>
-          <t>11827275.0</t>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>87</v>
+      </c>
+      <c r="L2" s="4" t="inlineStr">
+        <is>
+          <t>12062828.0</t>
         </is>
       </c>
     </row>
@@ -629,7 +621,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>17-DEC-24</t>
+          <t>26-DEC-24</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -638,14 +630,14 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G3" s="4" t="inlineStr">
         <is>
-          <t>299101.0</t>
-        </is>
-      </c>
-      <c r="H3" s="7" t="inlineStr">
+          <t>670500.0</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
@@ -659,67 +651,67 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L3" s="4" t="inlineStr">
         <is>
-          <t>299101.0</t>
+          <t>670500.0</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>SG - CAMEROUN</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>VISA INTERNATIONAL</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>ACHAT</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>17-DEC-24</t>
-        </is>
-      </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>26-DEC-24</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>XAF</t>
         </is>
       </c>
-      <c r="F4" s="5" t="n">
-        <v>359</v>
-      </c>
-      <c r="G4" s="6" t="inlineStr">
-        <is>
-          <t>32394490.0</t>
+      <c r="F4" t="n">
+        <v>326</v>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>23727938.0</t>
         </is>
       </c>
       <c r="H4" s="5" t="inlineStr">
         <is>
-          <t>not ok</t>
-        </is>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J4" s="6" t="inlineStr">
-        <is>
-          <t>6.0</t>
-        </is>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>353</v>
-      </c>
-      <c r="L4" s="6" t="inlineStr">
-        <is>
-          <t>32394484.0</t>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>326</v>
+      </c>
+      <c r="L4" s="4" t="inlineStr">
+        <is>
+          <t>23727938.0</t>
         </is>
       </c>
     </row>
@@ -741,7 +733,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17-DEC-24</t>
+          <t>26-DEC-24</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -750,14 +742,14 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="G5" s="4" t="inlineStr">
         <is>
-          <t>1960838.0</t>
-        </is>
-      </c>
-      <c r="H5" s="7" t="inlineStr">
+          <t>123670.0</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
@@ -771,11 +763,11 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="L5" s="4" t="inlineStr">
         <is>
-          <t>1960838.0</t>
+          <t>123670.0</t>
         </is>
       </c>
     </row>
@@ -797,7 +789,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>17-DEC-24</t>
+          <t>26-DEC-24</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -806,14 +798,14 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>633</v>
+        <v>448</v>
       </c>
       <c r="G6" s="4" t="inlineStr">
         <is>
-          <t>80126405.0</t>
-        </is>
-      </c>
-      <c r="H6" s="7" t="inlineStr">
+          <t>38584487.0</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
@@ -827,11 +819,11 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>633</v>
+        <v>448</v>
       </c>
       <c r="L6" s="4" t="inlineStr">
         <is>
-          <t>80126405.0</t>
+          <t>38584487.0</t>
         </is>
       </c>
     </row>
@@ -853,7 +845,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>17-DEC-24</t>
+          <t>26-DEC-24</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -862,14 +854,14 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
-          <t>92072937.0</t>
-        </is>
-      </c>
-      <c r="H7" s="7" t="inlineStr">
+          <t>138515480.0</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
@@ -883,11 +875,11 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="L7" s="4" t="inlineStr">
         <is>
-          <t>92072937.0</t>
+          <t>138515480.0</t>
         </is>
       </c>
     </row>
@@ -909,7 +901,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>17-DEC-24</t>
+          <t>26-DEC-24</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -918,14 +910,14 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>2851830.0</t>
-        </is>
-      </c>
-      <c r="H8" s="7" t="inlineStr">
+          <t>222517.0</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
@@ -939,11 +931,11 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="L8" s="4" t="inlineStr">
         <is>
-          <t>2851830.0</t>
+          <t>222517.0</t>
         </is>
       </c>
     </row>
@@ -965,7 +957,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>17-DEC-24</t>
+          <t>26-DEC-24</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -974,14 +966,14 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
-          <t>1548.2</t>
-        </is>
-      </c>
-      <c r="H9" s="7" t="inlineStr">
+          <t>401.0</t>
+        </is>
+      </c>
+      <c r="H9" s="5" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
@@ -995,11 +987,11 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>1548.2</t>
+          <t>401.0</t>
         </is>
       </c>
     </row>
@@ -1021,7 +1013,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>17-DEC-24</t>
+          <t>26-DEC-24</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1030,14 +1022,14 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>1330</v>
+        <v>1043</v>
       </c>
       <c r="G10" s="4" t="inlineStr">
         <is>
-          <t>439093418.0</t>
-        </is>
-      </c>
-      <c r="H10" s="7" t="inlineStr">
+          <t>370783584.0</t>
+        </is>
+      </c>
+      <c r="H10" s="5" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
@@ -1051,11 +1043,11 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>1330</v>
+        <v>1043</v>
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>439093418.0</t>
+          <t>370783584.0</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1069,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>17-DEC-24</t>
+          <t>26-DEC-24</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1086,14 +1078,14 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="G11" s="4" t="inlineStr">
         <is>
-          <t>94287000.0</t>
-        </is>
-      </c>
-      <c r="H11" s="7" t="inlineStr">
+          <t>2480000.0</t>
+        </is>
+      </c>
+      <c r="H11" s="5" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
@@ -1107,11 +1099,11 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="L11" s="4" t="inlineStr">
         <is>
-          <t>94287000.0</t>
+          <t>2480000.0</t>
         </is>
       </c>
     </row>
@@ -1126,14 +1118,9 @@
           <t>VISA INTERNATIONAL</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>ACHAT</t>
-        </is>
-      </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>17-DEC-24</t>
+          <t>26-DEC-24</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1142,14 +1129,14 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>543</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>53397119.0</t>
-        </is>
-      </c>
-      <c r="H12" s="7" t="inlineStr">
+          <t>200000.0</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
@@ -1163,18 +1150,18 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>543</v>
+        <v>1</v>
       </c>
       <c r="L12" s="4" t="inlineStr">
         <is>
-          <t>53397119.0</t>
+          <t>200000.0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SG - TCHAD</t>
+          <t>SG - SENEGAL</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1189,23 +1176,23 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>17-DEC-24</t>
+          <t>26-DEC-24</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>XAF</t>
+          <t>XOF</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>4</v>
+        <v>410</v>
       </c>
       <c r="G13" s="4" t="inlineStr">
         <is>
-          <t>97550.0</t>
-        </is>
-      </c>
-      <c r="H13" s="7" t="inlineStr">
+          <t>43761798.0</t>
+        </is>
+      </c>
+      <c r="H13" s="5" t="inlineStr">
         <is>
           <t>ok</t>
         </is>
@@ -1219,11 +1206,67 @@
         </is>
       </c>
       <c r="K13" t="n">
+        <v>410</v>
+      </c>
+      <c r="L13" s="4" t="inlineStr">
+        <is>
+          <t>43761798.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SG - TCHAD</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>VISA INTERNATIONAL</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ACHAT</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>26-DEC-24</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>XAF</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
         <v>4</v>
       </c>
-      <c r="L13" s="4" t="inlineStr">
-        <is>
-          <t>97550.0</t>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>145025.0</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="inlineStr">
+        <is>
+          <t>ok</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>4</v>
+      </c>
+      <c r="L14" s="4" t="inlineStr">
+        <is>
+          <t>145025.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update handle nbre de rejets 0
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -149,8 +149,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F5" headerRowCount="1">
-  <autoFilter ref="A1:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F4" headerRowCount="1">
+  <autoFilter ref="A1:F4"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Filiale"/>
     <tableColumn id="2" name="ARN"/>
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,11 +460,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="9" customWidth="1" min="5" max="5"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
     <col width="44" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -508,16 +508,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>74399724357101535635365</t>
+          <t>74399724366101545557798</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>21/12/2024</t>
+          <t>30/12/2024</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1149390</v>
+        <v>425115</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -531,19 +531,6 @@
           <t>SG - CAMEROUN</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>74399724365101544422581</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>29/12/2024</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>55000</v>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>V0202 POS Entry Mode is ** invalid</t>
@@ -553,22 +540,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SG - CAMEROUN</t>
-        </is>
+          <t>SG - COTE D IVOIRE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>74637414366101546447445</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TKNVHL</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>26/12/2024</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>92000</v>
       </c>
       <c r="F4" t="inlineStr">
-        <is>
-          <t>V0195 Authorization code is ****** invalid</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>SG - CAMEROUN</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
         <is>
           <t>V0202 POS Entry Mode is ** invalid</t>
         </is>

</xml_diff>

<commit_message>
fix 204 and 100 rejects
</commit_message>
<xml_diff>
--- a/styled_data.xlsx
+++ b/styled_data.xlsx
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>24000</v>
+        <v>24</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -606,7 +606,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>REJET EP</t>
+          <t>REJET VISA</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>54000</v>
+        <v>54</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -656,7 +656,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>REJET EP</t>
+          <t>REJET VISA</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">

</xml_diff>